<commit_message>
Realice las responsabilidades del modelo enriquesido de residentes y unos pequeños ajustes en el event storming de residentes
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Event Storming/Residentes - Event Storming.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Event Storming/Residentes - Event Storming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Event Storming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1EFED0-9F04-4B1C-8C72-85B51400FC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E69529A-5CD3-4802-8895-B63D1B08FECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
   <si>
     <t>Descripción</t>
   </si>
@@ -224,10 +224,13 @@
     <t>Se debe asegurar que no exista otro Residente registrado con el mismo numero de contacto.</t>
   </si>
   <si>
-    <t>Asegurar que el identificador del residente que se desea registrar  no ha haya sido asignado previamente a otro conjunto residencial.</t>
-  </si>
-  <si>
     <t>Se debe asegurar que no exista otro residente registrado con el mismo correo electronico.</t>
+  </si>
+  <si>
+    <t>Resid-Pol0005</t>
+  </si>
+  <si>
+    <t>Asegurar que el identificador del residente que se desea registrar  no ha haya sido asignado previamente a otro residente.</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -718,9 +721,57 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -730,6 +781,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -739,62 +799,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -802,8 +808,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1229,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02388B9D-0652-49D5-BF62-A59B793D6DFC}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1363,84 +1369,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="45" t="str">
+      <c r="B2" s="35" t="str">
         <f>'Listado Objetos de Dominio'!A6</f>
         <v>Inmueble</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="46"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="37" t="str">
         <f>'Listado Objetos de Dominio'!B6</f>
         <v xml:space="preserve">Objeto de dominio que representa el inmueble donde vive el residente del conjunto residencial. </v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="48"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="38"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50" t="s">
+      <c r="F4" s="40"/>
+      <c r="G4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="50"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1450,52 +1456,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="51" t="s">
+      <c r="L4" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="M4" s="43" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="53" t="s">
+      <c r="F5" s="40"/>
+      <c r="G5" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="55" t="s">
+      <c r="H5" s="44"/>
+      <c r="I5" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="K5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="51"/>
-      <c r="M5" s="52"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="43"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -1508,47 +1514,47 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="52"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="43"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="35" t="str">
+      <c r="B7" s="51" t="str">
         <f>_xlfn.CONCAT("Registrar ",B2)</f>
         <v>Registrar Inmueble</v>
       </c>
-      <c r="C7" s="35" t="str">
+      <c r="C7" s="51" t="str">
         <f>_xlfn.CONCAT("Acción de registrar un ",B2," para un conjunto residencial.")</f>
         <v>Acción de registrar un Inmueble para un conjunto residencial.</v>
       </c>
-      <c r="D7" s="35" t="str">
+      <c r="D7" s="51" t="str">
         <f>B2</f>
         <v>Inmueble</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35" t="str">
+      <c r="I7" s="51"/>
+      <c r="J7" s="51" t="str">
         <f>_xlfn.CONCAT(B2," registrado")</f>
         <v>Inmueble registrado</v>
       </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35" t="str">
+      <c r="K7" s="51"/>
+      <c r="L7" s="51" t="str">
         <f>_xlfn.CONCAT(B2," eliminado")</f>
         <v>Inmueble eliminado</v>
       </c>
@@ -1557,36 +1563,36 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="22" t="str">
         <f>_xlfn.CONCAT("Buscar ",B2)</f>
         <v>Buscar Inmueble</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
       <c r="M9" s="22" t="str">
         <f>_xlfn.CONCAT("Eliminar ",B2)</f>
         <v>Eliminar Inmueble</v>
@@ -1626,7 +1632,7 @@
         <v>Inmueble modificado</v>
       </c>
       <c r="K10" s="24"/>
-      <c r="L10" s="38" t="str">
+      <c r="L10" s="57" t="str">
         <f>_xlfn.CONCAT(B2," registrado")</f>
         <v>Inmueble registrado</v>
       </c>
@@ -1639,37 +1645,37 @@
       <c r="A11" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="35" t="str">
+      <c r="B11" s="51" t="str">
         <f>_xlfn.CONCAT("Buscar ",B2)</f>
         <v>Buscar Inmueble</v>
       </c>
-      <c r="C11" s="35" t="str">
+      <c r="C11" s="51" t="str">
         <f>_xlfn.CONCAT("Acción de buscar la información asociada a un ",B2," del conjunto residencial.")</f>
         <v>Acción de buscar la información asociada a un Inmueble del conjunto residencial.</v>
       </c>
-      <c r="D11" s="35" t="str">
+      <c r="D11" s="51" t="str">
         <f>B2</f>
         <v>Inmueble</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35" t="str">
+      <c r="I11" s="51"/>
+      <c r="J11" s="51" t="str">
         <f>_xlfn.CONCAT(B2," buscado")</f>
         <v>Inmueble buscado</v>
       </c>
-      <c r="K11" s="35"/>
-      <c r="L11" s="39"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="58"/>
       <c r="M11" s="22" t="str">
         <f>_xlfn.CONCAT("Modificar ",$B$2)</f>
         <v>Modificar Inmueble</v>
@@ -1679,17 +1685,17 @@
       <c r="A12" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="39"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="58"/>
       <c r="M12" s="26" t="str">
         <f>_xlfn.CONCAT("Eliminar ",$B$2)</f>
         <v>Eliminar Inmueble</v>
@@ -1729,7 +1735,7 @@
         <v>Inmueble eliminado</v>
       </c>
       <c r="K13" s="24"/>
-      <c r="L13" s="40"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="22" t="str">
         <f>_xlfn.CONCAT("Crear ",$B$2)</f>
         <v>Crear Inmueble</v>
@@ -1740,6 +1746,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -1756,30 +1786,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{171D8416-5555-47CC-88C6-059E12392622}"/>
@@ -1794,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEB74C4-8D06-495C-9F2F-FA132D609BF5}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1822,84 +1828,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="45" t="str">
+      <c r="B2" s="35" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Residente</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="46"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="37" t="str">
         <f>'Listado Objetos de Dominio'!B6</f>
         <v xml:space="preserve">Objeto de dominio que representa el inmueble donde vive el residente del conjunto residencial. </v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="48"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="38"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50" t="s">
+      <c r="F4" s="40"/>
+      <c r="G4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="50"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1909,52 +1915,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="51" t="s">
+      <c r="L4" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="M4" s="43" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="53" t="s">
+      <c r="F5" s="40"/>
+      <c r="G5" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="55" t="s">
+      <c r="H5" s="44"/>
+      <c r="I5" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="K5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="51"/>
-      <c r="M5" s="52"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="43"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -1967,47 +1973,47 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="52"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="43"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="35" t="str">
+      <c r="B7" s="51" t="str">
         <f>_xlfn.CONCAT("Registrar ",B2)</f>
         <v>Registrar Residente</v>
       </c>
-      <c r="C7" s="35" t="str">
+      <c r="C7" s="51" t="str">
         <f>_xlfn.CONCAT("Acción de registrar un ",B2," para un conjunto residencial.")</f>
         <v>Acción de registrar un Residente para un conjunto residencial.</v>
       </c>
-      <c r="D7" s="35" t="str">
+      <c r="D7" s="51" t="str">
         <f>B2</f>
         <v>Residente</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35" t="str">
+      <c r="I7" s="51"/>
+      <c r="J7" s="51" t="str">
         <f>_xlfn.CONCAT(B2," registrado")</f>
         <v>Residente registrado</v>
       </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35" t="str">
+      <c r="K7" s="51"/>
+      <c r="L7" s="51" t="str">
         <f>_xlfn.CONCAT(B2," eliminado")</f>
         <v>Residente eliminado</v>
       </c>
@@ -2016,36 +2022,36 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="22" t="str">
         <f>_xlfn.CONCAT("Buscar ",B2)</f>
         <v>Buscar Residente</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
       <c r="M9" s="22" t="str">
         <f>_xlfn.CONCAT("Eliminar ",B2)</f>
         <v>Eliminar Residente</v>
@@ -2085,7 +2091,7 @@
         <v>Residente modificado</v>
       </c>
       <c r="K10" s="24"/>
-      <c r="L10" s="38" t="str">
+      <c r="L10" s="57" t="str">
         <f>_xlfn.CONCAT(B2," registrado")</f>
         <v>Residente registrado</v>
       </c>
@@ -2095,60 +2101,62 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="35" t="str">
+      <c r="B11" s="51" t="str">
         <f>_xlfn.CONCAT("Buscar ",B2)</f>
         <v>Buscar Residente</v>
       </c>
-      <c r="C11" s="35" t="str">
+      <c r="C11" s="51" t="str">
         <f>_xlfn.CONCAT("Acción de buscar la información asociada a un ",B2," del conjunto residencial.")</f>
         <v>Acción de buscar la información asociada a un Residente del conjunto residencial.</v>
       </c>
-      <c r="D11" s="35" t="str">
+      <c r="D11" s="51" t="str">
         <f>B2</f>
         <v>Residente</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="63" t="s">
         <v>55</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35" t="str">
+      <c r="I11" s="51"/>
+      <c r="J11" s="51" t="str">
         <f>_xlfn.CONCAT(B2," buscado")</f>
         <v>Residente buscado</v>
       </c>
-      <c r="K11" s="35"/>
-      <c r="L11" s="39"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="58"/>
       <c r="M11" s="22" t="str">
         <f>_xlfn.CONCAT("Modificar ",$B$2)</f>
         <v>Modificar Residente</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="61"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="28" t="s">
+        <v>56</v>
+      </c>
       <c r="H12" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="39"/>
+        <v>62</v>
+      </c>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="58"/>
       <c r="M12" s="26" t="str">
         <f>_xlfn.CONCAT("Eliminar ",$B$2)</f>
         <v>Eliminar Residente</v>
@@ -2177,10 +2185,10 @@
         <v>36</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I13" s="24"/>
       <c r="J13" s="24" t="str">
@@ -2188,7 +2196,7 @@
         <v>Residente eliminado</v>
       </c>
       <c r="K13" s="24"/>
-      <c r="L13" s="40"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="22" t="str">
         <f>_xlfn.CONCAT("Crear ",$B$2)</f>
         <v>Crear Residente</v>
@@ -2198,7 +2206,34 @@
       <c r="E14" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="39">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2210,35 +2245,7 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{42C7641C-3E53-48C3-9D18-BDDC9B9DD3BA}"/>
@@ -2250,6 +2257,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C279D002CEC08F42B7087C30E58D0266" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5713f579c7011938dc4987ae8981b8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3219184d-29ab-4105-b29c-8e343e335d59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae0a0ff84a3c6712467f60982d6e378d" ns2:_="">
     <xsd:import namespace="3219184d-29ab-4105-b29c-8e343e335d59"/>
@@ -2393,35 +2415,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEECCE0-61F9-4782-94C5-382F8EFF459D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3219184d-29ab-4105-b29c-8e343e335d59"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2444,9 +2441,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEECCE0-61F9-4782-94C5-382F8EFF459D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3219184d-29ab-4105-b29c-8e343e335d59"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>